<commit_message>
added "legacy_column" field for information about the column name used in a legacy database if applicable
</commit_message>
<xml_diff>
--- a/lava-crms/development/instruments/datadictionary_template.xlsx
+++ b/lava-crms/development/instruments/datadictionary_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="12780" yWindow="480" windowWidth="28360" windowHeight="26080" tabRatio="814"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="71">
   <si>
     <t>instance</t>
   </si>
@@ -228,7 +228,10 @@
     <t>notes</t>
   </si>
   <si>
-    <t>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`) VALUES ('</t>
+    <t>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`,`legacy_column`) VALUES ('</t>
+  </si>
+  <si>
+    <t>legacy_column</t>
   </si>
 </sst>
 </file>
@@ -289,9 +292,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="428">
+  <cellStyleXfs count="432">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -724,7 +731,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="428">
+  <cellStyles count="432">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -938,6 +945,8 @@
     <cellStyle name="Followed Hyperlink" xfId="423" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="425" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="427" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="429" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="431" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -1152,6 +1161,8 @@
     <cellStyle name="Hyperlink" xfId="422" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="424" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="426" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="428" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="430" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1481,7 +1492,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <pane xSplit="7220" activePane="topRight"/>
@@ -1507,9 +1518,10 @@
     <col min="17" max="17" width="13.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1570,18 +1582,21 @@
       <c r="T1" t="s">
         <v>68</v>
       </c>
+      <c r="U1" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B2" s="1" t="str">
-        <f>D2 &amp; "','" &amp; E2 &amp; "','" &amp; F2 &amp; "','" &amp; G2 &amp; "','" &amp; H2 &amp; "','" &amp; I2 &amp; "','" &amp; J2 &amp; "','" &amp; K2 &amp; "','" &amp; L2 &amp; "','" &amp; M2 &amp; "','" &amp; N2 &amp; "','" &amp; O2 &amp; "','" &amp; P2 &amp; "','" &amp; Q2 &amp; "','" &amp; R2 &amp; "','" &amp; S2 &amp; "','" &amp; T2 &amp; "');"</f>
-        <v>lava','app-demo','entityname','1','propname1','1. This a full description of item 1.','1=Male; 2=Female','','1','tablename','columnname1','1','smallint','','1','null','');</v>
+        <f>D2 &amp; "','" &amp; E2 &amp; "','" &amp; F2 &amp; "','" &amp; G2 &amp; "','" &amp; H2 &amp; "','" &amp; I2 &amp; "','" &amp; J2 &amp; "','" &amp; K2 &amp; "','" &amp; L2 &amp; "','" &amp; M2 &amp; "','" &amp; N2 &amp; "','" &amp; O2 &amp; "','" &amp; P2 &amp; "','" &amp; Q2 &amp; "','" &amp; R2 &amp; "','" &amp; S2 &amp; "','" &amp; T2 &amp; "','" &amp; U2 &amp; "');"</f>
+        <v>lava','app-demo','entityname','1','propname1','1. This a full description of item 1.','1=Male; 2=Female','','1','tablename','columnname1','1','smallint','','1','null','','');</v>
       </c>
       <c r="C2" s="1" t="str">
         <f>A2 &amp; B2</f>
-        <v>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`) VALUES ('lava','app-demo','entityname','1','propname1','1. This a full description of item 1.','1=Male; 2=Female','','1','tablename','columnname1','1','smallint','','1','null','');</v>
+        <v>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`,`legacy_column`) VALUES ('lava','app-demo','entityname','1','propname1','1. This a full description of item 1.','1=Male; 2=Female','','1','tablename','columnname1','1','smallint','','1','null','','');</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -1629,17 +1644,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:21">
       <c r="A3" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B3" s="1" t="str">
-        <f t="shared" ref="B3:B11" si="0">D3 &amp; "','" &amp; E3 &amp; "','" &amp; F3 &amp; "','" &amp; G3 &amp; "','" &amp; H3 &amp; "','" &amp; I3 &amp; "','" &amp; J3 &amp; "','" &amp; K3 &amp; "','" &amp; L3 &amp; "','" &amp; M3 &amp; "','" &amp; N3 &amp; "','" &amp; O3 &amp; "','" &amp; P3 &amp; "','" &amp; Q3 &amp; "','" &amp; R3 &amp; "','" &amp; S3 &amp; "','" &amp; T3 &amp; "');"</f>
-        <v>lava','app-demo','entityname','2','propname2','2. This a full description of item 2.','0=No; 1=Yes','','1','tablename','columnname2','2','smallint','','1','null','');</v>
+        <f t="shared" ref="B3:B11" si="0">D3 &amp; "','" &amp; E3 &amp; "','" &amp; F3 &amp; "','" &amp; G3 &amp; "','" &amp; H3 &amp; "','" &amp; I3 &amp; "','" &amp; J3 &amp; "','" &amp; K3 &amp; "','" &amp; L3 &amp; "','" &amp; M3 &amp; "','" &amp; N3 &amp; "','" &amp; O3 &amp; "','" &amp; P3 &amp; "','" &amp; Q3 &amp; "','" &amp; R3 &amp; "','" &amp; S3 &amp; "','" &amp; T3 &amp; "','" &amp; U3 &amp; "');"</f>
+        <v>lava','app-demo','entityname','2','propname2','2. This a full description of item 2.','0=No; 1=Yes','','1','tablename','columnname2','2','smallint','','1','null','','');</v>
       </c>
       <c r="C3" s="1" t="str">
         <f t="shared" ref="C3:C11" si="1">A3 &amp; B3</f>
-        <v>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`) VALUES ('lava','app-demo','entityname','2','propname2','2. This a full description of item 2.','0=No; 1=Yes','','1','tablename','columnname2','2','smallint','','1','null','');</v>
+        <v>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`,`legacy_column`) VALUES ('lava','app-demo','entityname','2','propname2','2. This a full description of item 2.','0=No; 1=Yes','','1','tablename','columnname2','2','smallint','','1','null','','');</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -1687,17 +1702,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:21">
       <c r="A4" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>lava','app-demo','entityname','3','propname3','3. This a full description of item 3.','0=No; 1=Yes','','1','tablename','columnname3','3','smallint','','1','null','');</v>
+        <v>lava','app-demo','entityname','3','propname3','3. This a full description of item 3.','0=No; 1=Yes','','1','tablename','columnname3','3','smallint','','1','null','','');</v>
       </c>
       <c r="C4" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`) VALUES ('lava','app-demo','entityname','3','propname3','3. This a full description of item 3.','0=No; 1=Yes','','1','tablename','columnname3','3','smallint','','1','null','');</v>
+        <v>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`,`legacy_column`) VALUES ('lava','app-demo','entityname','3','propname3','3. This a full description of item 3.','0=No; 1=Yes','','1','tablename','columnname3','3','smallint','','1','null','','');</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -1742,17 +1757,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:21">
       <c r="A5" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>lava','app-demo','entityname','4','propname4','4. This a full description of item 4.','0=No; 1=Yes','','1','tablename','columnname4','4','smallint','','1','null','');</v>
+        <v>lava','app-demo','entityname','4','propname4','4. This a full description of item 4.','0=No; 1=Yes','','1','tablename','columnname4','4','smallint','','1','null','','');</v>
       </c>
       <c r="C5" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`) VALUES ('lava','app-demo','entityname','4','propname4','4. This a full description of item 4.','0=No; 1=Yes','','1','tablename','columnname4','4','smallint','','1','null','');</v>
+        <v>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`,`legacy_column`) VALUES ('lava','app-demo','entityname','4','propname4','4. This a full description of item 4.','0=No; 1=Yes','','1','tablename','columnname4','4','smallint','','1','null','','');</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -1800,17 +1815,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:21">
       <c r="A6" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>lava','app-demo','entityname','5','propname5','5. This a full description of item 5.','0=No; 1=Yes; 9=Unknown','','1','tablename','columnname5','5','smallint','','1','null','');</v>
+        <v>lava','app-demo','entityname','5','propname5','5. This a full description of item 5.','0=No; 1=Yes; 9=Unknown','','1','tablename','columnname5','5','smallint','','1','null','','');</v>
       </c>
       <c r="C6" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`) VALUES ('lava','app-demo','entityname','5','propname5','5. This a full description of item 5.','0=No; 1=Yes; 9=Unknown','','1','tablename','columnname5','5','smallint','','1','null','');</v>
+        <v>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`,`legacy_column`) VALUES ('lava','app-demo','entityname','5','propname5','5. This a full description of item 5.','0=No; 1=Yes; 9=Unknown','','1','tablename','columnname5','5','smallint','','1','null','','');</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -1858,17 +1873,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:21">
       <c r="A7" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>lava','app-demo','entityname','6','propname6','6. This a full description of item 6.','0-5','','1','tablename','columnname6','6','decimal','5,2','1','null','');</v>
+        <v>lava','app-demo','entityname','6','propname6','6. This a full description of item 6.','0-5','','1','tablename','columnname6','6','decimal','5,2','1','null','','');</v>
       </c>
       <c r="C7" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`) VALUES ('lava','app-demo','entityname','6','propname6','6. This a full description of item 6.','0-5','','1','tablename','columnname6','6','decimal','5,2','1','null','');</v>
+        <v>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`,`legacy_column`) VALUES ('lava','app-demo','entityname','6','propname6','6. This a full description of item 6.','0-5','','1','tablename','columnname6','6','decimal','5,2','1','null','','');</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -1916,17 +1931,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:21">
       <c r="A8" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>lava','app-demo','entityname','7','propname7','7. This a full description of item 7.','','','1','tablename','columnname7','7','varchar','255','1','null','');</v>
+        <v>lava','app-demo','entityname','7','propname7','7. This a full description of item 7.','','','1','tablename','columnname7','7','varchar','255','1','null','','');</v>
       </c>
       <c r="C8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`) VALUES ('lava','app-demo','entityname','7','propname7','7. This a full description of item 7.','','','1','tablename','columnname7','7','varchar','255','1','null','');</v>
+        <v>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`,`legacy_column`) VALUES ('lava','app-demo','entityname','7','propname7','7. This a full description of item 7.','','','1','tablename','columnname7','7','varchar','255','1','null','','');</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -1971,17 +1986,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:21">
       <c r="A9" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>lava','app-demo','entityname','8','propname8','8. This a full description of item 8.','0-10','','1','tablename','columnname8','8','smallint','','1','null','');</v>
+        <v>lava','app-demo','entityname','8','propname8','8. This a full description of item 8.','0-10','','1','tablename','columnname8','8','smallint','','1','null','','');</v>
       </c>
       <c r="C9" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`) VALUES ('lava','app-demo','entityname','8','propname8','8. This a full description of item 8.','0-10','','1','tablename','columnname8','8','smallint','','1','null','');</v>
+        <v>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`,`legacy_column`) VALUES ('lava','app-demo','entityname','8','propname8','8. This a full description of item 8.','0-10','','1','tablename','columnname8','8','smallint','','1','null','','');</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -2029,17 +2044,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:21">
       <c r="A10" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>lava','app-demo','entityname','9','propname9','9. This a full description of item 9.','0-20','','1','tablename','columnname9','9','smallint','','1','null','');</v>
+        <v>lava','app-demo','entityname','9','propname9','9. This a full description of item 9.','0-20','','1','tablename','columnname9','9','smallint','','1','null','','');</v>
       </c>
       <c r="C10" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`) VALUES ('lava','app-demo','entityname','9','propname9','9. This a full description of item 9.','0-20','','1','tablename','columnname9','9','smallint','','1','null','');</v>
+        <v>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`,`legacy_column`) VALUES ('lava','app-demo','entityname','9','propname9','9. This a full description of item 9.','0-20','','1','tablename','columnname9','9','smallint','','1','null','','');</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -2084,17 +2099,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:21">
       <c r="A11" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>lava','app-demo','entityname','10','propname10','10. This a full description of item 10.','0-30','propname8 + propname 9','1','tablename','columnname10','10','smallint','','1','null','');</v>
+        <v>lava','app-demo','entityname','10','propname10','10. This a full description of item 10.','0-30','propname8 + propname 9','1','tablename','columnname10','10','smallint','','1','null','','');</v>
       </c>
       <c r="C11" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`) VALUES ('lava','app-demo','entityname','10','propname10','10. This a full description of item 10.','0-30','propname8 + propname 9','1','tablename','columnname10','10','smallint','','1','null','');</v>
+        <v>INSERT INTO datadictionary (`instance`,`scope`,`entity`,`prop_order`,`prop_name`,`prop_description`,`data_values`,`data_calculation`,`required`,`db_table`,`db_column`,`db_order`,`db_datatype`,`db_datalength`,`db_nullable`,`db_default`,`notes`,`legacy_column`) VALUES ('lava','app-demo','entityname','10','propname10','10. This a full description of item 10.','0-30','propname8 + propname 9','1','tablename','columnname10','10','smallint','','1','null','','');</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>

</xml_diff>